<commit_message>
added some assertions to verizon test cases
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data.xlsx
+++ b/com.verizon/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.verizon\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FCD4E8-B2BE-4AE1-981C-3578359CA0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67E181B-ED9D-4507-8E2A-12292A522306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="628" firstSheet="7" activeTab="15" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
@@ -665,6 +665,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -717,7 +720,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -742,6 +745,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1625,10 +1629,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C97AC20-6DC1-48C5-9925-A1CA85849984}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1639,6 +1643,16 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18">
+        <v>19.989999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18">
+        <v>59.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5 Redfin TestCases pushed
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data.xlsx
+++ b/com.verizon/src/test/resources/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malik/IdeaProjects/Team1SeleniumBootcamp/com.verizon/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94C6296D-181F-F845-B71C-5A310A7E5993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3779E9DA-D0B7-D94A-AF68-32B811054137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="520" windowWidth="28040" windowHeight="16520" xr2:uid="{99EE0B41-9E9C-8D42-92B8-743B18628F08}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{D2C4DAFA-BAA9-E248-A90A-2B900FB98ACC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Sign-In</t>
-  </si>
-  <si>
-    <t>Verify your User ID or Mobile number is:</t>
+    <t>Motorola edge+ 5G UW</t>
   </si>
 </sst>
 </file>
@@ -389,26 +386,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60E84A74-A4ED-9D47-9318-AE70EE55564A}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82672C16-7297-D344-B1FF-655F60013720}">
+  <dimension ref="A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>